<commit_message>
don't use full names
</commit_message>
<xml_diff>
--- a/data/pop_bioinf_software.xlsx
+++ b/data/pop_bioinf_software.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="383">
   <si>
     <t xml:space="preserve">Karina</t>
   </si>
   <si>
-    <t xml:space="preserve">Brinkrolf</t>
+    <t xml:space="preserve">Br</t>
   </si>
   <si>
     <t xml:space="preserve">Datenquellen</t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Oliver</t>
   </si>
   <si>
-    <t xml:space="preserve">Schwengers</t>
+    <t xml:space="preserve">Sc</t>
   </si>
   <si>
     <t xml:space="preserve">AMRFinder</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Julian</t>
   </si>
   <si>
-    <t xml:space="preserve">Hahnfeld</t>
+    <t xml:space="preserve">Ha</t>
   </si>
   <si>
     <t xml:space="preserve">nan</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Linda</t>
   </si>
   <si>
-    <t xml:space="preserve">Fenske</t>
+    <t xml:space="preserve">Fe</t>
   </si>
   <si>
     <t xml:space="preserve">EBI</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Lukas</t>
   </si>
   <si>
-    <t xml:space="preserve">Jelonek</t>
+    <t xml:space="preserve">Je</t>
   </si>
   <si>
     <t xml:space="preserve">EDAM Ontology</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Patrick</t>
   </si>
   <si>
-    <t xml:space="preserve">Blumenkamp</t>
+    <t xml:space="preserve">Bl</t>
   </si>
   <si>
     <t xml:space="preserve">ENA</t>
@@ -94,16 +94,13 @@
     <t xml:space="preserve">Sebastian</t>
   </si>
   <si>
-    <t xml:space="preserve">Beyvers</t>
+    <t xml:space="preserve">Be</t>
   </si>
   <si>
     <t xml:space="preserve">Jochen</t>
   </si>
   <si>
-    <t xml:space="preserve">Blom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barth</t>
+    <t xml:space="preserve">Ba</t>
   </si>
   <si>
     <t xml:space="preserve">Ensembl</t>
@@ -127,7 +124,7 @@
     <t xml:space="preserve">Nina</t>
   </si>
   <si>
-    <t xml:space="preserve">Hofmann</t>
+    <t xml:space="preserve">Ho</t>
   </si>
   <si>
     <t xml:space="preserve">GO</t>
@@ -136,7 +133,7 @@
     <t xml:space="preserve">Anna</t>
   </si>
   <si>
-    <t xml:space="preserve">Rehm</t>
+    <t xml:space="preserve">Re</t>
   </si>
   <si>
     <t xml:space="preserve">Greengenes</t>
@@ -148,7 +145,7 @@
     <t xml:space="preserve">Sonja</t>
   </si>
   <si>
-    <t xml:space="preserve">Dietrich</t>
+    <t xml:space="preserve">Di</t>
   </si>
   <si>
     <t xml:space="preserve">IEDB (Immune Epitope Database)</t>
@@ -157,7 +154,7 @@
     <t xml:space="preserve">Sabine</t>
   </si>
   <si>
-    <t xml:space="preserve">Hurka</t>
+    <t xml:space="preserve">Hu</t>
   </si>
   <si>
     <t xml:space="preserve">InterproScan</t>
@@ -184,7 +181,7 @@
     <t xml:space="preserve">Katharina</t>
   </si>
   <si>
-    <t xml:space="preserve">Maibach</t>
+    <t xml:space="preserve">Ma</t>
   </si>
   <si>
     <t xml:space="preserve">miRecords</t>
@@ -253,7 +250,7 @@
     <t xml:space="preserve">sRNATarBase</t>
   </si>
   <si>
-    <t xml:space="preserve">Jaenicke</t>
+    <t xml:space="preserve">Ja</t>
   </si>
   <si>
     <t xml:space="preserve">SwissProt</t>
@@ -1363,11 +1360,11 @@
   </sheetPr>
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D82" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H121" activeCellId="0" sqref="H121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="43.78"/>
   </cols>
@@ -1554,7 +1551,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>2</v>
@@ -1571,16 +1568,16 @@
         <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,13 +1588,13 @@
         <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,7 +1614,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,13 +1625,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1651,7 +1648,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,7 +1668,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,19 +1676,19 @@
         <v>112</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,19 +1696,19 @@
         <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,13 +1719,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,16 +1733,16 @@
         <v>132</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,19 +1750,19 @@
         <v>80</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,16 +1770,16 @@
         <v>133</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="D22" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,11 +1787,11 @@
         <v>113</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D23" s="0" t="s">
         <v>2</v>
       </c>
@@ -1802,7 +1799,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,7 +1810,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>2</v>
@@ -1822,7 +1819,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,11 +1827,11 @@
         <v>111</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D25" s="0" t="s">
         <v>2</v>
       </c>
@@ -1842,7 +1839,7 @@
         <v>10</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,10 +1856,10 @@
         <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,7 +1879,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +1899,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,7 +1910,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>2</v>
@@ -1922,7 +1919,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,11 +1927,11 @@
         <v>105</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D30" s="0" t="s">
         <v>2</v>
       </c>
@@ -1942,7 +1939,7 @@
         <v>10</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,19 +1947,19 @@
         <v>103</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,11 +1967,11 @@
         <v>101</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D32" s="0" t="s">
         <v>2</v>
       </c>
@@ -1982,7 +1979,7 @@
         <v>10</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,7 +1999,7 @@
         <v>10</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2027,16 +2024,16 @@
         <v>135</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="D35" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,13 +2044,13 @@
         <v>25</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,11 +2058,11 @@
         <v>24</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D37" s="0" t="s">
         <v>2</v>
       </c>
@@ -2073,7 +2070,7 @@
         <v>10</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,7 +2090,7 @@
         <v>10</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2101,7 @@
         <v>20</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>2</v>
@@ -2113,7 +2110,7 @@
         <v>10</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2127,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,7 +2144,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,7 +2181,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,7 +2201,7 @@
         <v>10</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,11 +2209,11 @@
         <v>23</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D45" s="0" t="s">
         <v>2</v>
       </c>
@@ -2224,7 +2221,7 @@
         <v>10</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,11 +2229,11 @@
         <v>102</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D46" s="0" t="s">
         <v>2</v>
       </c>
@@ -2244,7 +2241,7 @@
         <v>10</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,7 +2261,7 @@
         <v>10</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,7 +2281,7 @@
         <v>10</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,13 +2292,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,7 +2315,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,7 +2326,7 @@
         <v>20</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>2</v>
@@ -2338,7 +2335,7 @@
         <v>10</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,11 +2343,11 @@
         <v>106</v>
       </c>
       <c r="B52" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D52" s="0" t="s">
         <v>2</v>
       </c>
@@ -2358,7 +2355,7 @@
         <v>10</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,7 +2389,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,7 +2406,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,7 +2417,7 @@
         <v>20</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>2</v>
@@ -2429,7 +2426,7 @@
         <v>10</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,11 +2434,11 @@
         <v>78</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D57" s="0" t="s">
         <v>2</v>
       </c>
@@ -2449,7 +2446,7 @@
         <v>10</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,7 +2466,7 @@
         <v>10</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2489,7 +2486,7 @@
         <v>10</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2497,11 +2494,11 @@
         <v>104</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D60" s="0" t="s">
         <v>2</v>
       </c>
@@ -2509,7 +2506,7 @@
         <v>10</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,16 +2517,16 @@
         <v>23</v>
       </c>
       <c r="C61" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2537,11 +2534,11 @@
         <v>79</v>
       </c>
       <c r="B62" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D62" s="0" t="s">
         <v>2</v>
       </c>
@@ -2549,7 +2546,7 @@
         <v>10</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2569,7 +2566,7 @@
         <v>10</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2577,16 +2574,16 @@
         <v>134</v>
       </c>
       <c r="B64" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C64" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="D64" s="0" t="s">
         <v>2</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2600,7 @@
         <v>2</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,7 +2617,7 @@
         <v>2</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,7 +2634,7 @@
         <v>2</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2648,28 +2645,28 @@
         <v>20</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D68" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E68" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="I68" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="I68" s="0" t="s">
+      <c r="J68" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="K68" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2683,25 +2680,25 @@
         <v>1</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E69" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="I69" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="I69" s="0" t="s">
+      <c r="J69" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="J69" s="0" t="s">
+      <c r="K69" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,25 +2712,25 @@
         <v>1</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E70" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="I70" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="I70" s="0" t="s">
+      <c r="J70" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="K70" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,25 +2744,25 @@
         <v>15</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F71" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I71" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="G71" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I71" s="0" t="s">
+      <c r="J71" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="K71" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,25 +2776,25 @@
         <v>15</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E72" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I72" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="G72" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I72" s="0" t="s">
+      <c r="J72" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="K72" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,28 +2805,28 @@
         <v>23</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F73" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G73" s="1" t="s">
+      <c r="I73" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="I73" s="0" t="s">
+      <c r="J73" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="K73" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,28 +2837,28 @@
         <v>23</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F74" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I74" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="G74" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I74" s="0" t="s">
+      <c r="J74" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,25 +2872,25 @@
         <v>21</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="I75" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="I75" s="0" t="s">
+      <c r="J75" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="K75" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="K75" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2907,25 +2904,25 @@
         <v>21</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E76" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="G76" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I76" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="G76" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I76" s="0" t="s">
+      <c r="J76" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="K76" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2933,31 +2930,31 @@
         <v>19</v>
       </c>
       <c r="B77" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C77" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D77" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F77" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I77" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="G77" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I77" s="0" t="s">
+      <c r="J77" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="K77" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2971,25 +2968,25 @@
         <v>21</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I78" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I78" s="0" t="s">
+      <c r="J78" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="K78" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2997,31 +2994,31 @@
         <v>75</v>
       </c>
       <c r="B79" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C79" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D79" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E79" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I79" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="G79" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I79" s="0" t="s">
+      <c r="J79" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="K79" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="80" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3029,31 +3026,31 @@
         <v>129</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D80" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F80" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G80" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G80" s="4" t="s">
+      <c r="H80" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I80" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H80" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="I80" s="3" t="s">
+      <c r="J80" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J80" s="5" t="s">
+      <c r="K80" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="K80" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,28 +3061,28 @@
         <v>23</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E81" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F81" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I81" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="G81" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I81" s="0" t="s">
+      <c r="J81" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="K81" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,28 +3093,28 @@
         <v>20</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I82" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="G82" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I82" s="0" t="s">
+      <c r="J82" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="K82" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="K82" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,22 +3128,22 @@
         <v>18</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G83" s="1" t="s">
+      <c r="I83" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="I83" s="0" t="s">
+      <c r="J83" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="K83" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="84" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3157,31 +3154,31 @@
         <v>23</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H84" s="3" t="n">
         <v>4</v>
       </c>
       <c r="I84" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J84" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="J84" s="3" t="s">
+      <c r="K84" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="K84" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3192,25 +3189,25 @@
         <v>25</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F85" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G85" s="1" t="s">
+      <c r="I85" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="I85" s="0" t="s">
+      <c r="J85" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J85" s="2" t="s">
+      <c r="K85" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3224,22 +3221,22 @@
         <v>6</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F86" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G86" s="1" t="s">
+      <c r="I86" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="I86" s="0" t="s">
+      <c r="J86" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J86" s="2" t="s">
+      <c r="K86" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3250,28 +3247,28 @@
         <v>20</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E87" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F87" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="I87" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="I87" s="0" t="s">
+      <c r="J87" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="K87" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="88" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3282,28 +3279,28 @@
         <v>25</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F88" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G88" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="H88" s="3" t="n">
         <v>3</v>
       </c>
       <c r="I88" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J88" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="J88" s="5" t="s">
+      <c r="K88" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3317,22 +3314,22 @@
         <v>6</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F89" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I89" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="G89" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I89" s="0" t="s">
+      <c r="J89" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="K89" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="K89" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3340,31 +3337,31 @@
         <v>100</v>
       </c>
       <c r="B90" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C90" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D90" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E90" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F90" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I90" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="G90" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="I90" s="0" t="s">
+      <c r="J90" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="J90" s="2" t="s">
+      <c r="K90" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3378,25 +3375,25 @@
         <v>15</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E91" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G91" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I91" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="I91" s="0" t="s">
+      <c r="J91" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="J91" s="2" t="s">
+      <c r="K91" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,22 +3407,22 @@
         <v>18</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F92" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G92" s="1" t="s">
+      <c r="I92" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="I92" s="0" t="s">
+      <c r="J92" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="J92" s="2" t="s">
+      <c r="K92" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="93" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,28 +3436,28 @@
         <v>9</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H93" s="3" t="n">
         <v>1</v>
       </c>
       <c r="I93" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="J93" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="J93" s="5" t="s">
+      <c r="K93" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="K93" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="94" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,34 +3465,34 @@
         <v>96</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D94" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H94" s="3" t="n">
         <v>8</v>
       </c>
       <c r="I94" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="J94" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="J94" s="5" t="s">
+      <c r="K94" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="K94" s="3" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3503,31 +3500,31 @@
         <v>99</v>
       </c>
       <c r="B95" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C95" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D95" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E95" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F95" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I95" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I95" s="0" t="s">
+      <c r="J95" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="J95" s="2" t="s">
+      <c r="K95" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="K95" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3535,31 +3532,31 @@
         <v>68</v>
       </c>
       <c r="B96" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C96" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D96" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E96" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F96" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I96" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="G96" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I96" s="0" t="s">
+      <c r="J96" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="J96" s="2" t="s">
+      <c r="K96" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="K96" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3570,28 +3567,28 @@
         <v>20</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E97" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F97" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I97" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="G97" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="I97" s="0" t="s">
+      <c r="J97" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="J97" s="2" t="s">
+      <c r="K97" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="K97" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3599,31 +3596,31 @@
         <v>110</v>
       </c>
       <c r="B98" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C98" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D98" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E98" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F98" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I98" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="G98" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I98" s="0" t="s">
+      <c r="J98" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="J98" s="0" t="s">
+      <c r="K98" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="99" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,34 +3628,34 @@
         <v>67</v>
       </c>
       <c r="B99" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D99" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F99" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H99" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I99" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="G99" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="H99" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I99" s="3" t="s">
+      <c r="J99" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="J99" s="5" t="s">
+      <c r="K99" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="K99" s="5" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="100" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,28 +3669,28 @@
         <v>24</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H100" s="3" t="n">
         <v>9</v>
       </c>
       <c r="I100" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J100" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="J100" s="5" t="s">
+      <c r="K100" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="K100" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,28 +3701,28 @@
         <v>23</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E101" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F101" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I101" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="G101" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I101" s="0" t="s">
+      <c r="J101" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="J101" s="2" t="s">
+      <c r="K101" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3736,28 +3733,28 @@
         <v>20</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E102" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F102" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I102" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="G102" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="I102" s="0" t="s">
+      <c r="J102" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J102" s="2" t="s">
+      <c r="K102" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,22 +3768,22 @@
         <v>6</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F103" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I103" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="G103" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I103" s="0" t="s">
+      <c r="J103" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="J103" s="2" t="s">
+      <c r="K103" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3800,25 +3797,25 @@
         <v>9</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E104" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F104" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I104" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="G104" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="I104" s="0" t="s">
+      <c r="J104" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="J104" s="2" t="s">
+      <c r="K104" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="105" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3832,28 +3829,28 @@
         <v>9</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H105" s="3" t="n">
         <v>7</v>
       </c>
       <c r="I105" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="J105" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="J105" s="5" t="s">
+      <c r="K105" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="K105" s="5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3867,25 +3864,25 @@
         <v>1</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F106" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I106" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="G106" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="I106" s="0" t="s">
+      <c r="J106" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="J106" s="2" t="s">
+      <c r="K106" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3899,25 +3896,25 @@
         <v>9</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E107" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F107" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I107" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="G107" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="I107" s="0" t="s">
+      <c r="J107" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="J107" s="2" t="s">
+      <c r="K107" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,25 +3928,25 @@
         <v>21</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F108" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I108" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="G108" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="I108" s="0" t="s">
+      <c r="J108" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="J108" s="2" t="s">
+      <c r="K108" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3963,25 +3960,25 @@
         <v>21</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F109" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G109" s="1" t="s">
+      <c r="I109" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="I109" s="0" t="s">
+      <c r="J109" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="J109" s="2" t="s">
+      <c r="K109" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="K109" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3995,25 +3992,25 @@
         <v>21</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E110" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="G110" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I110" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="G110" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="I110" s="0" t="s">
+      <c r="J110" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="J110" s="2" t="s">
+      <c r="K110" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="K110" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4027,28 +4024,28 @@
         <v>21</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E111" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F111" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G111" s="1" t="s">
+      <c r="I111" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="I111" s="0" t="s">
+      <c r="J111" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="J111" s="2" t="s">
+      <c r="K111" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="K111" s="2" t="s">
+      <c r="L111" s="0" t="s">
         <v>276</v>
-      </c>
-      <c r="L111" s="0" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4062,25 +4059,25 @@
         <v>24</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F112" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I112" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="G112" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I112" s="1" t="s">
+      <c r="J112" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J112" s="2" t="s">
+      <c r="K112" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="K112" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="113" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4094,25 +4091,25 @@
         <v>6</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H113" s="3" t="n">
         <v>5</v>
       </c>
       <c r="I113" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J113" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="J113" s="5" t="s">
+      <c r="K113" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="K113" s="5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4126,25 +4123,25 @@
         <v>21</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F114" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I114" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="G114" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="I114" s="0" t="s">
+      <c r="J114" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="J114" s="2" t="s">
+      <c r="K114" s="0" t="s">
         <v>288</v>
-      </c>
-      <c r="K114" s="0" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4158,25 +4155,25 @@
         <v>21</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F115" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I115" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="G115" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="I115" s="0" t="s">
+      <c r="J115" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="J115" s="2" t="s">
+      <c r="K115" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,31 +4181,31 @@
         <v>76</v>
       </c>
       <c r="B116" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C116" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C116" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D116" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E116" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F116" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="I116" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="G116" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="I116" s="0" t="s">
+      <c r="J116" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="J116" s="2" t="s">
+      <c r="K116" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="K116" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4222,25 +4219,25 @@
         <v>21</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F117" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="I117" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="I117" s="0" t="s">
+      <c r="J117" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="J117" s="2" t="s">
+      <c r="K117" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4251,28 +4248,28 @@
         <v>23</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E118" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F118" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I118" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="G118" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="I118" s="0" t="s">
+      <c r="J118" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="J118" s="0" t="s">
+      <c r="K118" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="K118" s="2" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,25 +4283,25 @@
         <v>9</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E119" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F119" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I119" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="G119" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I119" s="0" t="s">
+      <c r="J119" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="J119" s="2" t="s">
+      <c r="K119" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="K119" s="2" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="120" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4312,32 +4309,32 @@
         <v>98</v>
       </c>
       <c r="B120" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C120" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D120" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H120" s="0"/>
       <c r="I120" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="J120" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="J120" s="5" t="s">
+      <c r="K120" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="K120" s="5" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4345,34 +4342,34 @@
         <v>97</v>
       </c>
       <c r="B121" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C121" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C121" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D121" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E121" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F121" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H121" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="G121" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="H121" s="3" t="s">
+      <c r="I121" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="I121" s="0" t="s">
-        <v>317</v>
-      </c>
       <c r="J121" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="K121" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="K121" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4380,34 +4377,34 @@
         <v>69</v>
       </c>
       <c r="B122" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C122" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D122" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E122" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F122" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G122" s="1" t="s">
+      <c r="I122" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="I122" s="0" t="s">
+      <c r="J122" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="J122" s="2" t="s">
+      <c r="K122" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="K122" s="0" t="s">
+      <c r="L122" s="0" t="s">
         <v>322</v>
-      </c>
-      <c r="L122" s="0" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4415,34 +4412,34 @@
         <v>22</v>
       </c>
       <c r="B123" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C123" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C123" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D123" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E123" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F123" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I123" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="G123" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="I123" s="0" t="s">
+      <c r="J123" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="J123" s="2" t="s">
+      <c r="K123" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="K123" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="L123" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4450,34 +4447,34 @@
         <v>21</v>
       </c>
       <c r="B124" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C124" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C124" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D124" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E124" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F124" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="I124" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="G124" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="I124" s="0" t="s">
+      <c r="J124" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="J124" s="2" t="s">
+      <c r="K124" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="K124" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="L124" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4485,34 +4482,34 @@
         <v>77</v>
       </c>
       <c r="B125" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C125" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C125" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D125" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E125" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F125" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="I125" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="G125" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="I125" s="0" t="s">
+      <c r="J125" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="J125" s="2" t="s">
+      <c r="K125" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="K125" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="L125" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,25 +4523,25 @@
         <v>9</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E126" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F126" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I126" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="G126" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="I126" s="0" t="s">
+      <c r="J126" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="J126" s="2" t="s">
+      <c r="K126" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="K126" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4552,31 +4549,31 @@
         <v>131</v>
       </c>
       <c r="B127" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C127" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C127" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="D127" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F127" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="I127" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="G127" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="I127" s="0" t="s">
+      <c r="J127" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="J127" s="2" t="s">
+      <c r="K127" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="K127" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="L127" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,22 +4587,22 @@
         <v>18</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F128" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="I128" s="0" t="s">
         <v>344</v>
       </c>
-      <c r="G128" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="I128" s="0" t="s">
+      <c r="J128" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="J128" s="2" t="s">
+      <c r="K128" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="K128" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,25 +4616,25 @@
         <v>9</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E129" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F129" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="I129" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="G129" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="I129" s="0" t="s">
+      <c r="J129" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="J129" s="2" t="s">
+      <c r="K129" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="K129" s="2" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4645,34 +4642,34 @@
         <v>18</v>
       </c>
       <c r="B130" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C130" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C130" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D130" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E130" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F130" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I130" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="G130" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="I130" s="0" t="s">
+      <c r="J130" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="J130" s="2" t="s">
+      <c r="K130" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="K130" s="2" t="s">
+      <c r="L130" s="0" t="s">
         <v>355</v>
-      </c>
-      <c r="L130" s="0" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,31 +4677,31 @@
         <v>20</v>
       </c>
       <c r="B131" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C131" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C131" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D131" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E131" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F131" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="I131" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="G131" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="I131" s="0" t="s">
+      <c r="J131" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="J131" s="2" t="s">
+      <c r="K131" s="0" t="s">
         <v>359</v>
-      </c>
-      <c r="K131" s="0" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4718,25 +4715,25 @@
         <v>1</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F132" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="I132" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="I132" s="0" t="s">
+      <c r="J132" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="J132" s="2" t="s">
-        <v>364</v>
-      </c>
       <c r="K132" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4750,25 +4747,25 @@
         <v>1</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F133" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="I133" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="I133" s="0" t="s">
+      <c r="J133" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="J133" s="2" t="s">
-        <v>368</v>
-      </c>
       <c r="K133" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4776,28 +4773,28 @@
         <v>128</v>
       </c>
       <c r="B134" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C134" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C134" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="D134" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F134" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I134" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="G134" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="I134" s="0" t="s">
+      <c r="J134" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="J134" s="2" t="s">
-        <v>371</v>
-      </c>
       <c r="K134" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4808,19 +4805,19 @@
         <v>20</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E135" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4828,22 +4825,22 @@
         <v>73</v>
       </c>
       <c r="B136" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C136" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C136" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D136" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E136" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4857,16 +4854,16 @@
         <v>9</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E137" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,16 +4874,16 @@
         <v>25</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4897,19 +4894,19 @@
         <v>20</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E139" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G139" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4923,16 +4920,16 @@
         <v>24</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E140" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G140" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4940,22 +4937,22 @@
         <v>70</v>
       </c>
       <c r="B141" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C141" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C141" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D141" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E141" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G141" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4969,16 +4966,16 @@
         <v>1</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G142" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4989,16 +4986,16 @@
         <v>25</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G143" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5012,13 +5009,13 @@
         <v>6</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5029,19 +5026,19 @@
         <v>20</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E145" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5049,22 +5046,22 @@
         <v>66</v>
       </c>
       <c r="B146" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C146" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C146" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D146" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E146" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5072,22 +5069,22 @@
         <v>109</v>
       </c>
       <c r="B147" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C147" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C147" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D147" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E147" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5101,16 +5098,16 @@
         <v>9</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E148" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5118,19 +5115,19 @@
         <v>130</v>
       </c>
       <c r="B149" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C149" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C149" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="D149" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5144,13 +5141,13 @@
         <v>6</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5164,16 +5161,16 @@
         <v>15</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E151" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5187,16 +5184,16 @@
         <v>1</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5207,16 +5204,16 @@
         <v>25</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5224,22 +5221,22 @@
         <v>65</v>
       </c>
       <c r="B154" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C154" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C154" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D154" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E154" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5253,16 +5250,16 @@
         <v>1</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5276,16 +5273,16 @@
         <v>21</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5296,19 +5293,19 @@
         <v>20</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E157" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5316,22 +5313,22 @@
         <v>108</v>
       </c>
       <c r="B158" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C158" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C158" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D158" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E158" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5345,13 +5342,13 @@
         <v>18</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5359,22 +5356,22 @@
         <v>71</v>
       </c>
       <c r="B160" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C160" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C160" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D160" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E160" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F160" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5388,13 +5385,13 @@
         <v>6</v>
       </c>
       <c r="D161" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5408,13 +5405,13 @@
         <v>18</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5428,13 +5425,13 @@
         <v>6</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5448,13 +5445,13 @@
         <v>6</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5468,16 +5465,16 @@
         <v>1</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E165" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5491,16 +5488,16 @@
         <v>21</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E166" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F166" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G166" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5511,19 +5508,19 @@
         <v>23</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E167" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5534,19 +5531,19 @@
         <v>20</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E168" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5554,22 +5551,22 @@
         <v>72</v>
       </c>
       <c r="B169" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C169" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C169" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D169" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E169" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5577,22 +5574,22 @@
         <v>74</v>
       </c>
       <c r="B170" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C170" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C170" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D170" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E170" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,19 +5600,19 @@
         <v>20</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E171" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5623,22 +5620,22 @@
         <v>107</v>
       </c>
       <c r="B172" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C172" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C172" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D172" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E172" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5649,19 +5646,19 @@
         <v>20</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E173" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>